<commit_message>
Modificado libro de responsabilidades
</commit_message>
<xml_diff>
--- a/responsabilidades.xlsx
+++ b/responsabilidades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROPIETARIO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROPIETARIO\Documents\Git\Reingenieria\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Por hacer</t>
   </si>
@@ -584,7 +584,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -634,11 +634,11 @@
         <v>8</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="13"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="1"/>
       <c r="H6" s="2"/>
       <c r="K6" t="s">
         <v>4</v>
@@ -652,11 +652,11 @@
         <v>11</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="1"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -667,7 +667,9 @@
         <v>12</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="F8" s="12"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
@@ -680,7 +682,9 @@
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>

</xml_diff>

<commit_message>
Modificado documento y libro de responsabilidades
</commit_message>
<xml_diff>
--- a/responsabilidades.xlsx
+++ b/responsabilidades.xlsx
@@ -584,7 +584,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -667,11 +667,11 @@
         <v>12</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="14"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificado modulo de inicio
</commit_message>
<xml_diff>
--- a/responsabilidades.xlsx
+++ b/responsabilidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Por hacer</t>
   </si>
@@ -584,7 +584,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -682,11 +682,11 @@
         <v>13</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -697,7 +697,9 @@
         <v>14</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="F10" s="12"/>
       <c r="G10" s="14"/>
       <c r="H10" s="2"/>
@@ -710,7 +712,9 @@
         <v>15</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="2"/>

</xml_diff>